<commit_message>
Commit version 1.1 bug fixes
</commit_message>
<xml_diff>
--- a/dataUpload/dataTemplates/Templates/Accounting_Opening_Balances.xlsx
+++ b/dataUpload/dataTemplates/Templates/Accounting_Opening_Balances.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">Chart of Account Name</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">Credit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
   </si>
 </sst>
 </file>
@@ -214,10 +217,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -227,7 +230,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="6" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="7" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
@@ -246,6 +250,9 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="1048012" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>